<commit_message>
last changes to excel file
</commit_message>
<xml_diff>
--- a/speedup_report.xlsx
+++ b/speedup_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RobertoCarlos\Downloads\multiprocesadores\euler_pi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298A5DB2-7023-4128-9333-DAF7D1218A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DA3CDE-24A2-46F1-9D4F-32B3ECF5FD32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,25 +86,25 @@
     <t>Tiempos en milisegundos (ms)</t>
   </si>
   <si>
-    <t>OpenMPspeedup</t>
+    <t>Iterations</t>
   </si>
   <si>
-    <t>CUDAspeedup</t>
+    <t>OpenMP-speedup</t>
   </si>
   <si>
-    <t>TBBSpeedup</t>
+    <t>CUDA-speedup</t>
   </si>
   <si>
-    <t>Threadsspeedup</t>
+    <t>TBB-speedup</t>
   </si>
   <si>
-    <t>ForkJoinspeedup</t>
+    <t>Threads-speedup</t>
   </si>
   <si>
-    <t>GoroutinesSpeedup</t>
+    <t>ForkJoin-speedup</t>
   </si>
   <si>
-    <t>Iterations</t>
+    <t>Goroutines-speedup</t>
   </si>
 </sst>
 </file>
@@ -182,14 +182,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,7 +559,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2708,7 +2707,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>OpenMPspeedup</c:v>
+                  <c:v>OpenMP-speedup</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2788,7 +2787,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TBBSpeedup</c:v>
+                  <c:v>TBB-speedup</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2868,7 +2867,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Threadsspeedup</c:v>
+                  <c:v>Threads-speedup</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2948,7 +2947,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ForkJoinspeedup</c:v>
+                  <c:v>ForkJoin-speedup</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3028,7 +3027,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>GoroutinesSpeedup</c:v>
+                  <c:v>Goroutines-speedup</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3128,7 +3127,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>CUDAspeedup</c:v>
+                        <c:v>CUDA-speedup</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -6719,8 +6718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFD90CD-9C14-43A9-904C-38E2B43B58B9}">
   <dimension ref="B3:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V29" sqref="V29"/>
+    <sheetView tabSelected="1" topLeftCell="M9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI20" sqref="AI20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6735,41 +6734,41 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="4" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="4" t="s">
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="4" t="s">
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>0</v>
@@ -6781,14 +6780,14 @@
         <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>1</v>
@@ -6797,11 +6796,11 @@
         <v>4</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="M4" s="4"/>
       <c r="N4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>2</v>
@@ -6813,14 +6812,14 @@
         <v>6</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="T4" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="T4" s="4"/>
       <c r="U4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="V4" s="3" t="s">
         <v>14</v>
@@ -6829,7 +6828,7 @@
         <v>7</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.3">
@@ -7108,7 +7107,7 @@
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>1532.6877999999999</v>
       </c>
       <c r="D9" s="1">
@@ -7173,7 +7172,7 @@
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
excel file serial-graphs finished
</commit_message>
<xml_diff>
--- a/speedup_report.xlsx
+++ b/speedup_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RobertoCarlos\Downloads\multiprocesadores\euler_pi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DA3CDE-24A2-46F1-9D4F-32B3ECF5FD32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EAB04D-090C-47E4-B906-DE1ED50739BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3514,6 +3514,1486 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX"/>
+              <a:t>Serial implementations</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Times!$B$5:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1x10^4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1x10^5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1x10^6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1x10^7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1x10^8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$C$5:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.41959999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7999000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.4674</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>157.11199999999999</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="#,##0.00">
+                  <c:v>1532.6877999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-03E4-466D-9F7C-9D343EEA9584}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C++</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Times!$B$5:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1x10^4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1x10^5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1x10^6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1x10^7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1x10^8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$J$5:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.374</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4908000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.747900000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>236.833</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2373.42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-03E4-466D-9F7C-9D343EEA9584}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$O$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Java</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Times!$B$5:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1x10^4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1x10^5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1x10^6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1x10^7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1x10^8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$O$5:$O$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>323.39999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3242.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-03E4-466D-9F7C-9D343EEA9584}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$V$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Golang</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Times!$B$5:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1x10^4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1x10^5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1x10^6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1x10^7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1x10^8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$V$5:$V$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.9395</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.9161999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>112.0645</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1018.3721</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10897.6999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-03E4-466D-9F7C-9D343EEA9584}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1408582895"/>
+        <c:axId val="1408593711"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1408582895"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1408593711"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1408593711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Execution Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1408582895"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX"/>
+              <a:t>Concurrent</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-MX" baseline="0"/>
+              <a:t> implementations</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>OpenMP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Times!$U$5:$U$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1x10^4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1x10^5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1x10^6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1x10^7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1x10^8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$D$5:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.29210000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6202999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.183700000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-993A-44E2-8C61-C4B7580E68BE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CUDA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Times!$U$5:$U$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1x10^4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1x10^5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1x10^6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1x10^7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1x10^8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$E$5:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.1000000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8999999999999998E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-993A-44E2-8C61-C4B7580E68BE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$P$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Threads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Times!$U$5:$U$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1x10^4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1x10^5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1x10^6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1x10^7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1x10^8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$P$5:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>629.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-993A-44E2-8C61-C4B7580E68BE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$Q$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ForkJoin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Times!$U$5:$U$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1x10^4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1x10^5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1x10^6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1x10^7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1x10^8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$Q$5:$Q$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>631</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-993A-44E2-8C61-C4B7580E68BE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Times!$W$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Goroutines</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Times!$U$5:$U$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1x10^4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1x10^5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1x10^6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1x10^7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1x10^8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Times!$W$5:$W$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.33439999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1360000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.619199999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>226.2636</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2404.7984000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-993A-44E2-8C61-C4B7580E68BE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1183838655"/>
+        <c:axId val="1183839071"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1183838655"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Iterations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1183839071"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1183839071"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Execution</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> Time (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1183838655"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3714,6 +5194,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -5753,6 +7313,1038 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6450,6 +9042,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC58A245-4533-055F-D600-CF1E350153A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D03F7CA-7A5E-909E-46B2-81D322FBD8E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6718,8 +9382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFD90CD-9C14-43A9-904C-38E2B43B58B9}">
   <dimension ref="B3:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI20" sqref="AI20"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>